<commit_message>
implemented printing of invoice
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\FlixLLCPL\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B66ECE-98D6-41FB-A96C-FA335E458D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425D99DA-16FB-4FDE-9F17-B2147B684710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="3060" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
+    <workbookView xWindow="8415" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="__I__">Sheet1!$A$14:$AL$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -110,15 +111,16 @@
     <t>&lt;#Number&gt;</t>
   </si>
   <si>
-    <t>&lt;#DueDate&gt;</t>
+    <t>&lt;#DueOn&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -350,22 +352,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="10" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,89 +410,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -836,7 +843,7 @@
   <dimension ref="A2:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,22 +855,22 @@
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="40" t="s">
+      <c r="Y2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="40"/>
-      <c r="AJ2" s="40"/>
-      <c r="AK2" s="40"/>
-      <c r="AL2" s="40"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F3" s="2" t="s">
@@ -875,20 +882,20 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="Y3" s="40"/>
-      <c r="Z3" s="40"/>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="40"/>
-      <c r="AC3" s="40"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="40"/>
-      <c r="AG3" s="40"/>
-      <c r="AH3" s="40"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="40"/>
-      <c r="AK3" s="40"/>
-      <c r="AL3" s="40"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="28"/>
+      <c r="AJ3" s="28"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
     </row>
     <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F4" s="2" t="s">
@@ -900,20 +907,20 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
-      <c r="AI4" s="40"/>
-      <c r="AJ4" s="40"/>
-      <c r="AK4" s="40"/>
-      <c r="AL4" s="40"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="28"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="28"/>
+      <c r="AL4" s="28"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -937,298 +944,298 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="31"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="33"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="34"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="33"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="34"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="33"/>
-      <c r="T10" s="37" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="34"/>
+      <c r="T10" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38" t="s">
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38" t="s">
+      <c r="AB10" s="27"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="38"/>
-      <c r="AJ10" s="38"/>
-      <c r="AK10" s="38"/>
+      <c r="AG10" s="27"/>
+      <c r="AH10" s="27"/>
+      <c r="AI10" s="27"/>
+      <c r="AJ10" s="27"/>
+      <c r="AK10" s="27"/>
       <c r="AL10" s="39"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="36"/>
-      <c r="T11" s="27" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="37"/>
+      <c r="T11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="24" t="s">
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="24"/>
-      <c r="AD11" s="24"/>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="25" t="s">
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AG11" s="25"/>
-      <c r="AH11" s="25"/>
-      <c r="AI11" s="25"/>
-      <c r="AJ11" s="25"/>
-      <c r="AK11" s="25"/>
-      <c r="AL11" s="26"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="12"/>
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="13"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6" t="s">
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="38" t="s">
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AG13" s="38"/>
-      <c r="AH13" s="38"/>
-      <c r="AI13" s="38"/>
-      <c r="AJ13" s="38"/>
-      <c r="AK13" s="38"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
+      <c r="AK13" s="27"/>
       <c r="AL13" s="39"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="7" t="s">
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="7" t="s">
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="19" t="s">
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="16"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AG14" s="20"/>
-      <c r="AH14" s="20"/>
-      <c r="AI14" s="20"/>
-      <c r="AJ14" s="20"/>
-      <c r="AK14" s="20"/>
-      <c r="AL14" s="21"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="8"/>
     </row>
-    <row r="15" spans="1:38" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="13" t="s">
+    <row r="15" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="22" t="s">
+      <c r="AA15" s="41"/>
+      <c r="AB15" s="41"/>
+      <c r="AC15" s="41"/>
+      <c r="AD15" s="41"/>
+      <c r="AE15" s="41"/>
+      <c r="AF15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AG15" s="22"/>
-      <c r="AH15" s="22"/>
-      <c r="AI15" s="22"/>
-      <c r="AJ15" s="22"/>
-      <c r="AK15" s="22"/>
-      <c r="AL15" s="23"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+      <c r="AL15" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
     <mergeCell ref="Y2:AL4"/>
     <mergeCell ref="B7:R11"/>
     <mergeCell ref="A13:B13"/>
@@ -1247,6 +1254,9 @@
     <mergeCell ref="Z15:AE15"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:T14"/>
+    <mergeCell ref="Z13:AE13"/>
+    <mergeCell ref="U13:Y13"/>
+    <mergeCell ref="C13:T13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adjusted invoice address for postal
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\FlixLLCPL\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425D99DA-16FB-4FDE-9F17-B2147B684710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00F35CC-EB7F-4BB3-BD57-951924BB8AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8415" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="__I__">Sheet1!$A$14:$AL$14</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$13</definedName>
+    <definedName name="__I__">Sheet1!$A$15:$AL$15</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -352,13 +352,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -410,6 +449,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,51 +467,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -840,10 +848,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AL15"/>
+  <dimension ref="A2:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,22 +863,22 @@
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="Y2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F3" s="2" t="s">
@@ -882,20 +890,20 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="28"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
     </row>
     <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F4" s="2" t="s">
@@ -907,356 +915,379 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="28"/>
-      <c r="AJ4" s="28"/>
-      <c r="AK4" s="28"/>
-      <c r="AL4" s="28"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="5"/>
+    <row r="5" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="34"/>
+    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="12"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="34"/>
+    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="12"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="34"/>
-      <c r="T10" s="38" t="s">
+    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="12"/>
+      <c r="T11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AA10" s="27" t="s">
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="27"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27" t="s">
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="27"/>
-      <c r="AL10" s="39"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="17"/>
+      <c r="AJ11" s="17"/>
+      <c r="AK11" s="17"/>
+      <c r="AL11" s="18"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="37"/>
-      <c r="T11" s="14" t="s">
+    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="15"/>
+      <c r="T12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="11" t="s">
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="12" t="s">
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AG11" s="12"/>
-      <c r="AH11" s="12"/>
-      <c r="AI11" s="12"/>
-      <c r="AJ11" s="12"/>
-      <c r="AK11" s="12"/>
-      <c r="AL11" s="13"/>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="25"/>
+      <c r="AJ12" s="25"/>
+      <c r="AK12" s="25"/>
+      <c r="AL12" s="26"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27" t="s">
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27" t="s">
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="27"/>
-      <c r="AI13" s="27"/>
-      <c r="AJ13" s="27"/>
-      <c r="AK13" s="27"/>
-      <c r="AL13" s="39"/>
+      <c r="AG14" s="17"/>
+      <c r="AH14" s="17"/>
+      <c r="AI14" s="17"/>
+      <c r="AJ14" s="17"/>
+      <c r="AK14" s="17"/>
+      <c r="AL14" s="18"/>
     </row>
-    <row r="14" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+    <row r="15" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="18" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="15" t="s">
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="16"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="17"/>
-      <c r="AF14" s="6" t="s">
+      <c r="AA15" s="29"/>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="29"/>
+      <c r="AD15" s="29"/>
+      <c r="AE15" s="30"/>
+      <c r="AF15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="8"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+      <c r="AI15" s="20"/>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="20"/>
+      <c r="AL15" s="21"/>
     </row>
-    <row r="15" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="40" t="s">
+    <row r="16" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="34"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
-      <c r="AD15" s="41"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="9" t="s">
+      <c r="AA16" s="37"/>
+      <c r="AB16" s="37"/>
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="37"/>
+      <c r="AE16" s="37"/>
+      <c r="AF16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
-      <c r="AL15" s="10"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="22"/>
+      <c r="AI16" s="22"/>
+      <c r="AJ16" s="22"/>
+      <c r="AK16" s="22"/>
+      <c r="AL16" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="Y2:AL4"/>
-    <mergeCell ref="B7:R11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AF13:AL13"/>
-    <mergeCell ref="T10:Z10"/>
-    <mergeCell ref="AF10:AL10"/>
-    <mergeCell ref="AA10:AE10"/>
-    <mergeCell ref="AF14:AL14"/>
     <mergeCell ref="AF15:AL15"/>
-    <mergeCell ref="AA11:AE11"/>
-    <mergeCell ref="AF11:AL11"/>
-    <mergeCell ref="T11:Z11"/>
+    <mergeCell ref="AF16:AL16"/>
+    <mergeCell ref="AA12:AE12"/>
+    <mergeCell ref="AF12:AL12"/>
+    <mergeCell ref="T12:Z12"/>
+    <mergeCell ref="Z15:AE15"/>
+    <mergeCell ref="U15:Y15"/>
+    <mergeCell ref="A16:Y16"/>
+    <mergeCell ref="Z16:AE16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:T15"/>
     <mergeCell ref="Z14:AE14"/>
     <mergeCell ref="U14:Y14"/>
-    <mergeCell ref="A15:Y15"/>
-    <mergeCell ref="Z15:AE15"/>
+    <mergeCell ref="C14:T14"/>
+    <mergeCell ref="D8:R12"/>
+    <mergeCell ref="Y2:AL4"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:T14"/>
-    <mergeCell ref="Z13:AE13"/>
-    <mergeCell ref="U13:Y13"/>
-    <mergeCell ref="C13:T13"/>
+    <mergeCell ref="AF14:AL14"/>
+    <mergeCell ref="T11:Z11"/>
+    <mergeCell ref="AF11:AL11"/>
+    <mergeCell ref="AA11:AE11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
improved invoice, added preview, multiline
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\FlixLLCPL\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00F35CC-EB7F-4BB3-BD57-951924BB8AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D7B9ED-FEFF-41D3-83E0-171E964B1A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8415" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>&lt;#I.Idx&gt;</t>
   </si>
   <si>
-    <t>&lt;#I.Title&gt;</t>
-  </si>
-  <si>
     <t>&lt;#I.Quantity&gt;</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>&lt;#DueOn&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#I.Title&gt;&lt;#Row Height(autofit)&gt;</t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,12 +139,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Black"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
@@ -194,6 +188,18 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -352,93 +358,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -449,32 +429,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -851,7 +856,7 @@
   <dimension ref="A2:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="AP14" sqref="AP14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,411 +864,408 @@
     <col min="1" max="72" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F2" s="1" t="s">
+    <row r="2" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
     </row>
     <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.35">
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
     </row>
     <row r="5" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="10"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="34"/>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="12"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="37"/>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="12"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="37"/>
     </row>
     <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="12"/>
-      <c r="T11" s="16" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="37"/>
+      <c r="T11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="17" t="s">
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17" t="s">
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AG11" s="17"/>
-      <c r="AH11" s="17"/>
-      <c r="AI11" s="17"/>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="18"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="12"/>
     </row>
-    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="15"/>
-      <c r="T12" s="27" t="s">
+    <row r="12" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="40"/>
+      <c r="T12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="24" t="s">
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="16"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
-      <c r="AI12" s="25"/>
-      <c r="AJ12" s="25"/>
-      <c r="AK12" s="25"/>
-      <c r="AL12" s="26"/>
+      <c r="AG12" s="17"/>
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="17"/>
+      <c r="AK12" s="17"/>
+      <c r="AL12" s="18"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="17"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="17"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="17" t="s">
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AA14" s="17"/>
-      <c r="AB14" s="17"/>
-      <c r="AC14" s="17"/>
-      <c r="AD14" s="17"/>
-      <c r="AE14" s="17"/>
-      <c r="AF14" s="17" t="s">
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AG14" s="17"/>
-      <c r="AH14" s="17"/>
-      <c r="AI14" s="17"/>
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="17"/>
-      <c r="AL14" s="18"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="12"/>
     </row>
     <row r="15" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="31" t="s">
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="21"/>
+      <c r="AD15" s="21"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA15" s="29"/>
-      <c r="AB15" s="29"/>
-      <c r="AC15" s="29"/>
-      <c r="AD15" s="29"/>
-      <c r="AE15" s="30"/>
-      <c r="AF15" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG15" s="20"/>
-      <c r="AH15" s="20"/>
-      <c r="AI15" s="20"/>
-      <c r="AJ15" s="20"/>
-      <c r="AK15" s="20"/>
-      <c r="AL15" s="21"/>
+      <c r="AG15" s="14"/>
+      <c r="AH15" s="14"/>
+      <c r="AI15" s="14"/>
+      <c r="AJ15" s="14"/>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="15"/>
     </row>
     <row r="16" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="34"/>
-      <c r="W16" s="34"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="36" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA16" s="42"/>
+      <c r="AB16" s="42"/>
+      <c r="AC16" s="42"/>
+      <c r="AD16" s="42"/>
+      <c r="AE16" s="42"/>
+      <c r="AF16" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="AA16" s="37"/>
-      <c r="AB16" s="37"/>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="37"/>
-      <c r="AE16" s="37"/>
-      <c r="AF16" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="22"/>
-      <c r="AI16" s="22"/>
-      <c r="AJ16" s="22"/>
-      <c r="AK16" s="22"/>
-      <c r="AL16" s="23"/>
+      <c r="AG16" s="43"/>
+      <c r="AH16" s="43"/>
+      <c r="AI16" s="43"/>
+      <c r="AJ16" s="43"/>
+      <c r="AK16" s="43"/>
+      <c r="AL16" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="21">

</xml_diff>

<commit_message>
fixed major bug with form sizing
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\FlixLLCPL\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D7B9ED-FEFF-41D3-83E0-171E964B1A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DE2109-68D9-4FF1-B398-F5A18BFB894F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Invoice &lt;#Number&gt;" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="__I__">Sheet1!$A$15:$AL$15</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$14</definedName>
+    <definedName name="__I__">'Invoice &lt;#Number&gt;'!$A$15:$AL$15</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Invoice &lt;#Number&gt;'!$1:$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -182,13 +182,6 @@
       <family val="3"/>
     </font>
     <font>
-      <u val="singleAccounting"/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -199,6 +192,13 @@
       <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -370,115 +370,115 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -856,7 +856,7 @@
   <dimension ref="A2:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP14" sqref="AP14"/>
+      <selection activeCell="AJ24" sqref="AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,22 +868,22 @@
       <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+      <c r="AL2" s="24"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F3" s="7" t="s">
@@ -895,20 +895,20 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
     </row>
     <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F4" s="7" t="s">
@@ -920,20 +920,20 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
     </row>
     <row r="5" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F5" s="1"/>
@@ -979,296 +979,302 @@
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="6"/>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="34"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="37"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="20"/>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="20"/>
     </row>
     <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="37"/>
-      <c r="T11" s="10" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="20"/>
+      <c r="T11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11" t="s">
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11" t="s">
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11"/>
-      <c r="AL11" s="12"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="14"/>
+      <c r="AJ11" s="14"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="26"/>
     </row>
     <row r="12" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="40"/>
-      <c r="T12" s="19" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="23"/>
+      <c r="T12" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="U12" s="17"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="17"/>
-      <c r="X12" s="17"/>
-      <c r="Y12" s="17"/>
-      <c r="Z12" s="17"/>
-      <c r="AA12" s="16" t="s">
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="17" t="s">
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AG12" s="17"/>
-      <c r="AH12" s="17"/>
-      <c r="AI12" s="17"/>
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
-      <c r="AL12" s="18"/>
+      <c r="AG12" s="42"/>
+      <c r="AH12" s="42"/>
+      <c r="AI12" s="42"/>
+      <c r="AJ12" s="42"/>
+      <c r="AK12" s="42"/>
+      <c r="AL12" s="44"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11" t="s">
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11" t="s">
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AL14" s="12"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="26"/>
     </row>
     <row r="15" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="23" t="s">
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="20" t="s">
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="22"/>
-      <c r="AF15" s="13" t="s">
+      <c r="AA15" s="36"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="36"/>
+      <c r="AD15" s="36"/>
+      <c r="AE15" s="37"/>
+      <c r="AF15" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AG15" s="14"/>
-      <c r="AH15" s="14"/>
-      <c r="AI15" s="14"/>
-      <c r="AJ15" s="14"/>
-      <c r="AK15" s="14"/>
-      <c r="AL15" s="15"/>
+      <c r="AG15" s="39"/>
+      <c r="AH15" s="39"/>
+      <c r="AI15" s="39"/>
+      <c r="AJ15" s="39"/>
+      <c r="AK15" s="39"/>
+      <c r="AL15" s="40"/>
     </row>
     <row r="16" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="41" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AA16" s="42"/>
-      <c r="AB16" s="42"/>
-      <c r="AC16" s="42"/>
-      <c r="AD16" s="42"/>
-      <c r="AE16" s="42"/>
-      <c r="AF16" s="43" t="s">
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="13"/>
+      <c r="AF16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AG16" s="43"/>
-      <c r="AH16" s="43"/>
-      <c r="AI16" s="43"/>
-      <c r="AJ16" s="43"/>
-      <c r="AK16" s="43"/>
-      <c r="AL16" s="44"/>
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
+      <c r="AI16" s="27"/>
+      <c r="AJ16" s="27"/>
+      <c r="AK16" s="27"/>
+      <c r="AL16" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Y2:AL4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="AF14:AL14"/>
+    <mergeCell ref="T11:Z11"/>
+    <mergeCell ref="AF11:AL11"/>
+    <mergeCell ref="AA11:AE11"/>
     <mergeCell ref="AF15:AL15"/>
     <mergeCell ref="AF16:AL16"/>
     <mergeCell ref="AA12:AE12"/>
@@ -1284,12 +1290,6 @@
     <mergeCell ref="U14:Y14"/>
     <mergeCell ref="C14:T14"/>
     <mergeCell ref="D8:R12"/>
-    <mergeCell ref="Y2:AL4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="AF14:AL14"/>
-    <mergeCell ref="T11:Z11"/>
-    <mergeCell ref="AF11:AL11"/>
-    <mergeCell ref="AA11:AE11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added template for profit/loss
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flixllcpl\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79049F05-294E-49BA-AFDB-644DFC9CEFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2BE43C-F531-4696-B994-257339D9F7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34590" windowHeight="18555" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
@@ -16,8 +16,9 @@
     <sheet name="Invoice &lt;#Number&gt;" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="__I__">'Invoice &lt;#Number&gt;'!$A$15:$AL$15</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Invoice &lt;#Number&gt;'!$1:$14</definedName>
+    <definedName name="__I__">'Invoice &lt;#Number&gt;'!$A$14:$AL$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Invoice &lt;#Number&gt;'!$A:$AL</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Invoice &lt;#Number&gt;'!$1:$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -350,7 +351,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -447,37 +450,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -504,13 +507,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>15587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -853,10 +856,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AL16"/>
+  <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF15" sqref="AF15:AL15"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,13 +867,38 @@
     <col min="1" max="72" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F2" s="8" t="s">
+    <row r="1" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+    </row>
+    <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.35">
+      <c r="F2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
       <c r="AB2" s="9"/>
@@ -887,7 +915,7 @@
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F3" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -910,92 +938,86 @@
       <c r="AK3" s="9"/>
       <c r="AL3" s="9"/>
     </row>
-    <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.35">
-      <c r="F4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+    <row r="4" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
     </row>
-    <row r="5" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5"/>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="4"/>
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="26"/>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="29"/>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
@@ -1034,265 +1056,246 @@
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="29"/>
+      <c r="T10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="12"/>
     </row>
-    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="29"/>
-      <c r="T11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11"/>
-      <c r="AL11" s="12"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="32"/>
+      <c r="T11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG11" s="16"/>
+      <c r="AH11" s="16"/>
+      <c r="AI11" s="16"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="17"/>
     </row>
-    <row r="12" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="32"/>
-      <c r="T12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="16"/>
-      <c r="AJ12" s="16"/>
-      <c r="AK12" s="16"/>
-      <c r="AL12" s="17"/>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="12"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AL14" s="12"/>
+    <row r="14" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="V14" s="38"/>
+      <c r="W14" s="38"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA14" s="40"/>
+      <c r="AB14" s="40"/>
+      <c r="AC14" s="40"/>
+      <c r="AD14" s="40"/>
+      <c r="AE14" s="41"/>
+      <c r="AF14" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG14" s="43"/>
+      <c r="AH14" s="43"/>
+      <c r="AI14" s="43"/>
+      <c r="AJ14" s="43"/>
+      <c r="AK14" s="43"/>
+      <c r="AL14" s="44"/>
     </row>
-    <row r="15" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="V15" s="38"/>
-      <c r="W15" s="38"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA15" s="40"/>
-      <c r="AB15" s="40"/>
-      <c r="AC15" s="40"/>
-      <c r="AD15" s="40"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG15" s="43"/>
-      <c r="AH15" s="43"/>
-      <c r="AI15" s="43"/>
-      <c r="AJ15" s="43"/>
-      <c r="AK15" s="43"/>
-      <c r="AL15" s="44"/>
-    </row>
-    <row r="16" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="20"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="20"/>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="22" t="s">
+    <row r="15" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="13" t="s">
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="23"/>
+      <c r="AE15" s="23"/>
+      <c r="AF15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AG16" s="13"/>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="13"/>
-      <c r="AJ16" s="13"/>
-      <c r="AK16" s="13"/>
-      <c r="AL16" s="14"/>
+      <c r="AG15" s="13"/>
+      <c r="AH15" s="13"/>
+      <c r="AI15" s="13"/>
+      <c r="AJ15" s="13"/>
+      <c r="AK15" s="13"/>
+      <c r="AL15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AF14:AL14"/>
     <mergeCell ref="AF15:AL15"/>
-    <mergeCell ref="AF16:AL16"/>
-    <mergeCell ref="AA12:AE12"/>
-    <mergeCell ref="AF12:AL12"/>
-    <mergeCell ref="T12:Z12"/>
-    <mergeCell ref="Z15:AE15"/>
-    <mergeCell ref="U15:Y15"/>
-    <mergeCell ref="A16:Y16"/>
-    <mergeCell ref="Z16:AE16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:T15"/>
+    <mergeCell ref="AA11:AE11"/>
+    <mergeCell ref="AF11:AL11"/>
+    <mergeCell ref="T11:Z11"/>
     <mergeCell ref="Z14:AE14"/>
     <mergeCell ref="U14:Y14"/>
+    <mergeCell ref="A15:Y15"/>
+    <mergeCell ref="Z15:AE15"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:T14"/>
-    <mergeCell ref="D8:R12"/>
-    <mergeCell ref="Y2:AL4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="AF14:AL14"/>
-    <mergeCell ref="T11:Z11"/>
-    <mergeCell ref="AF11:AL11"/>
-    <mergeCell ref="AA11:AE11"/>
+    <mergeCell ref="Z13:AE13"/>
+    <mergeCell ref="U13:Y13"/>
+    <mergeCell ref="C13:T13"/>
+    <mergeCell ref="D7:R11"/>
+    <mergeCell ref="Y1:AL3"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="AF13:AL13"/>
+    <mergeCell ref="T10:Z10"/>
+    <mergeCell ref="AF10:AL10"/>
+    <mergeCell ref="AA10:AE10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="99" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated invoice template with new field name
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flixllcpl\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2BE43C-F531-4696-B994-257339D9F7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A27B1DE-0EEA-4E44-B314-F9ED9027BA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="34590" windowHeight="18555" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="24060" windowHeight="13095" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice &lt;#Number&gt;" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <t>&lt;#DueOn&gt;</t>
   </si>
   <si>
-    <t>&lt;#I.Title&gt;&lt;#Row Height(autofit)&gt;</t>
+    <t>&lt;#I.Description&gt;&lt;#Row Height(autofit)&gt;</t>
   </si>
 </sst>
 </file>
@@ -375,113 +375,113 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -859,7 +859,7 @@
   <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+      <selection activeCell="A15" sqref="A15:Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,22 +871,22 @@
       <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="42"/>
+      <c r="AK1" s="42"/>
+      <c r="AL1" s="42"/>
     </row>
     <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F2" s="7" t="s">
@@ -898,20 +898,20 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="42"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
+      <c r="AJ2" s="42"/>
+      <c r="AK2" s="42"/>
+      <c r="AL2" s="42"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F3" s="7" t="s">
@@ -923,20 +923,20 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42"/>
+      <c r="AA3" s="42"/>
+      <c r="AB3" s="42"/>
+      <c r="AC3" s="42"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="42"/>
+      <c r="AF3" s="42"/>
+      <c r="AG3" s="42"/>
+      <c r="AH3" s="42"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
     </row>
     <row r="4" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4" s="1"/>
@@ -982,296 +982,302 @@
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="26"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="35"/>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="29"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="38"/>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="29"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="38"/>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="29"/>
-      <c r="T10" s="10" t="s">
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="38"/>
+      <c r="T10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11" t="s">
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11" t="s">
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="32"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="32"/>
+      <c r="AF10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="11"/>
-      <c r="AJ10" s="11"/>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="12"/>
+      <c r="AG10" s="32"/>
+      <c r="AH10" s="32"/>
+      <c r="AI10" s="32"/>
+      <c r="AJ10" s="32"/>
+      <c r="AK10" s="32"/>
+      <c r="AL10" s="44"/>
     </row>
     <row r="11" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="32"/>
-      <c r="T11" s="18" t="s">
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="41"/>
+      <c r="T11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="15" t="s">
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="16" t="s">
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
-      <c r="AI11" s="16"/>
-      <c r="AJ11" s="16"/>
-      <c r="AK11" s="16"/>
-      <c r="AL11" s="17"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="16"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11" t="s">
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11" t="s">
+      <c r="AA13" s="32"/>
+      <c r="AB13" s="32"/>
+      <c r="AC13" s="32"/>
+      <c r="AD13" s="32"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="12"/>
+      <c r="AG13" s="32"/>
+      <c r="AH13" s="32"/>
+      <c r="AI13" s="32"/>
+      <c r="AJ13" s="32"/>
+      <c r="AK13" s="32"/>
+      <c r="AL13" s="44"/>
     </row>
     <row r="14" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="37" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="V14" s="38"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="39" t="s">
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="AA14" s="40"/>
-      <c r="AB14" s="40"/>
-      <c r="AC14" s="40"/>
-      <c r="AD14" s="40"/>
-      <c r="AE14" s="41"/>
-      <c r="AF14" s="42" t="s">
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AG14" s="43"/>
-      <c r="AH14" s="43"/>
-      <c r="AI14" s="43"/>
-      <c r="AJ14" s="43"/>
-      <c r="AK14" s="43"/>
-      <c r="AL14" s="44"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="10"/>
+      <c r="AJ14" s="10"/>
+      <c r="AK14" s="10"/>
+      <c r="AL14" s="11"/>
     </row>
     <row r="15" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="22" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="25"/>
+      <c r="Z15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-      <c r="AE15" s="23"/>
-      <c r="AF15" s="13" t="s">
+      <c r="AA15" s="27"/>
+      <c r="AB15" s="27"/>
+      <c r="AC15" s="27"/>
+      <c r="AD15" s="27"/>
+      <c r="AE15" s="27"/>
+      <c r="AF15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AG15" s="13"/>
-      <c r="AH15" s="13"/>
-      <c r="AI15" s="13"/>
-      <c r="AJ15" s="13"/>
-      <c r="AK15" s="13"/>
-      <c r="AL15" s="14"/>
+      <c r="AG15" s="12"/>
+      <c r="AH15" s="12"/>
+      <c r="AI15" s="12"/>
+      <c r="AJ15" s="12"/>
+      <c r="AK15" s="12"/>
+      <c r="AL15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Y1:AL3"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="AF13:AL13"/>
+    <mergeCell ref="T10:Z10"/>
+    <mergeCell ref="AF10:AL10"/>
+    <mergeCell ref="AA10:AE10"/>
     <mergeCell ref="AF14:AL14"/>
     <mergeCell ref="AF15:AL15"/>
     <mergeCell ref="AA11:AE11"/>
@@ -1287,12 +1293,6 @@
     <mergeCell ref="U13:Y13"/>
     <mergeCell ref="C13:T13"/>
     <mergeCell ref="D7:R11"/>
-    <mergeCell ref="Y1:AL3"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AF13:AL13"/>
-    <mergeCell ref="T10:Z10"/>
-    <mergeCell ref="AF10:AL10"/>
-    <mergeCell ref="AA10:AE10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="99" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated template and invoice printer
</commit_message>
<xml_diff>
--- a/vcl/src/templates/Invoice.xlsx
+++ b/vcl/src/templates/Invoice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flixaccounting.templates\Generic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\flixaccounting\vcl\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B5C4E-E9FE-4E0D-AE4A-8DEAC53D77F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFD4941-1156-49E2-A770-0EF0B6B5A891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="25350" windowHeight="13260" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
+    <workbookView xWindow="25395" yWindow="11250" windowWidth="28800" windowHeight="15345" xr2:uid="{C51E7660-53A8-4CD8-8974-FD3CBFE2CB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice &lt;#Number&gt;" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <t>&lt;#CompanyAddressLine&gt;</t>
   </si>
   <si>
-    <t>&lt;#CompanyCityZip&gt;</t>
+    <t>&lt;#CompanyCityZipLine&gt;</t>
   </si>
 </sst>
 </file>
@@ -375,6 +375,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -444,9 +456,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -473,15 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -861,7 +861,7 @@
   <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,22 +873,22 @@
       <c r="F1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="42" t="s">
+      <c r="Y1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AI1" s="42"/>
-      <c r="AJ1" s="42"/>
-      <c r="AK1" s="42"/>
-      <c r="AL1" s="42"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
     </row>
     <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F2" s="7" t="s">
@@ -900,20 +900,20 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="42"/>
-      <c r="AI2" s="42"/>
-      <c r="AJ2" s="42"/>
-      <c r="AK2" s="42"/>
-      <c r="AL2" s="42"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.35">
       <c r="F3" s="7" t="s">
@@ -925,20 +925,20 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="42"/>
-      <c r="AH3" s="42"/>
-      <c r="AI3" s="42"/>
-      <c r="AJ3" s="42"/>
-      <c r="AK3" s="42"/>
-      <c r="AL3" s="42"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
     </row>
     <row r="4" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4" s="1"/>
@@ -984,302 +984,296 @@
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="35"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="38"/>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="41"/>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="41"/>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="38"/>
-      <c r="T10" s="43" t="s">
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="41"/>
+      <c r="T10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32" t="s">
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="32"/>
-      <c r="AD10" s="32"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="32" t="s">
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AG10" s="32"/>
-      <c r="AH10" s="32"/>
-      <c r="AI10" s="32"/>
-      <c r="AJ10" s="32"/>
-      <c r="AK10" s="32"/>
-      <c r="AL10" s="44"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="12"/>
     </row>
     <row r="11" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="41"/>
-      <c r="T11" s="17" t="s">
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="44"/>
+      <c r="T11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="14" t="s">
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="15" t="s">
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AG11" s="15"/>
-      <c r="AH11" s="15"/>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="15"/>
-      <c r="AK11" s="15"/>
-      <c r="AL11" s="16"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="20"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32" t="s">
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32"/>
-      <c r="AC13" s="32"/>
-      <c r="AD13" s="32"/>
-      <c r="AE13" s="32"/>
-      <c r="AF13" s="32" t="s">
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AG13" s="32"/>
-      <c r="AH13" s="32"/>
-      <c r="AI13" s="32"/>
-      <c r="AJ13" s="32"/>
-      <c r="AK13" s="32"/>
-      <c r="AL13" s="44"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="12"/>
     </row>
     <row r="14" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="21" t="s">
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="18" t="s">
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
-      <c r="AC14" s="19"/>
-      <c r="AD14" s="19"/>
-      <c r="AE14" s="20"/>
-      <c r="AF14" s="9" t="s">
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="11"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="15"/>
     </row>
     <row r="15" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="26" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="27"/>
-      <c r="AD15" s="27"/>
-      <c r="AE15" s="27"/>
-      <c r="AF15" s="12" t="s">
+      <c r="AA15" s="31"/>
+      <c r="AB15" s="31"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="31"/>
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AG15" s="12"/>
-      <c r="AH15" s="12"/>
-      <c r="AI15" s="12"/>
-      <c r="AJ15" s="12"/>
-      <c r="AK15" s="12"/>
-      <c r="AL15" s="13"/>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="16"/>
+      <c r="AJ15" s="16"/>
+      <c r="AK15" s="16"/>
+      <c r="AL15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="Y1:AL3"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AF13:AL13"/>
-    <mergeCell ref="T10:Z10"/>
-    <mergeCell ref="AF10:AL10"/>
-    <mergeCell ref="AA10:AE10"/>
     <mergeCell ref="AF14:AL14"/>
     <mergeCell ref="AF15:AL15"/>
     <mergeCell ref="AA11:AE11"/>
@@ -1295,6 +1289,12 @@
     <mergeCell ref="U13:Y13"/>
     <mergeCell ref="C13:T13"/>
     <mergeCell ref="D7:R11"/>
+    <mergeCell ref="Y1:AL3"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="AF13:AL13"/>
+    <mergeCell ref="T10:Z10"/>
+    <mergeCell ref="AF10:AL10"/>
+    <mergeCell ref="AA10:AE10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="99" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>